<commit_message>
long time no see, commit to be, we'll see you thee, the time for me may last at tea, while none come free, yet all may see the true of me
</commit_message>
<xml_diff>
--- a/IsignTransverse_ETH/results/block_size.xlsx
+++ b/IsignTransverse_ETH/results/block_size.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafałŚwiętek(236668)\source\repos\IsignTransverse\IsignTransverse_ETH\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4175E2-D340-4A04-B9EF-7B8C81EBB363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307D6F07-D3CD-43A4-8F00-1FB7132EB349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CFB5EDEB-8AEB-4285-A041-E73EA331D414}"/>
+    <workbookView xWindow="0" yWindow="1176" windowWidth="17280" windowHeight="8964" xr2:uid="{CFB5EDEB-8AEB-4285-A041-E73EA331D414}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="21">
   <si>
     <t>L</t>
   </si>
@@ -87,6 +87,39 @@
   </si>
   <si>
     <t>k=3*2π/L</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>l.nonzero</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>program</t>
   </si>
 </sst>
 </file>
@@ -154,7 +187,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -272,11 +305,20 @@
         <color indexed="64"/>
       </diagonal>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -286,17 +328,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -312,6 +345,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -319,11 +390,7 @@
   <dxfs count="15">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -335,29 +402,6 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -418,6 +462,27 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -522,19 +587,11 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </font>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -552,11 +609,25 @@
       </font>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-      </border>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1974,13 +2045,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>385380</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>341586</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>533926</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>181654</xdr:rowOff>
@@ -2012,7 +2083,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B29F9A13-323A-43D8-A7AD-9B92576D2C32}" name="Tabela2" displayName="Tabela2" ref="C5:H17" totalsRowShown="0" headerRowDxfId="1" dataDxfId="13" tableBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B29F9A13-323A-43D8-A7AD-9B92576D2C32}" name="Tabela2" displayName="Tabela2" ref="C5:H17" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="C5:H17" xr:uid="{B29F9A13-323A-43D8-A7AD-9B92576D2C32}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D1D9FB0A-4EE6-4EF9-AE69-C051D64BF2C1}" name="L" dataDxfId="11"/>
@@ -2029,13 +2100,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1E9F6556-4DAB-4947-A3E6-10DA2051B482}" name="Tabela3" displayName="Tabela3" ref="I5:L17" totalsRowShown="0" headerRowDxfId="0" dataDxfId="12">
-  <autoFilter ref="I5:L17" xr:uid="{1E9F6556-4DAB-4947-A3E6-10DA2051B482}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1E9F6556-4DAB-4947-A3E6-10DA2051B482}" name="Tabela3" displayName="Tabela3" ref="J5:M17" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="J5:M17" xr:uid="{1E9F6556-4DAB-4947-A3E6-10DA2051B482}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DF1B1051-5BFE-4B19-A90B-6A429C3597D6}" name="+1,+1" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{4FD9D15B-A45D-457D-B949-B229736A3386}" name="+1,-1" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{C9DEAC31-FA7F-417E-A128-80EC5E6FCDA2}" name="-1,+1" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{4211D2A8-F9C3-4FBB-AFB6-20CD367E3889}" name="-1,-1" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{DF1B1051-5BFE-4B19-A90B-6A429C3597D6}" name="+1,+1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{4FD9D15B-A45D-457D-B949-B229736A3386}" name="+1,-1" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{C9DEAC31-FA7F-417E-A128-80EC5E6FCDA2}" name="-1,+1" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{4211D2A8-F9C3-4FBB-AFB6-20CD367E3889}" name="-1,-1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2338,87 +2409,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEB2813-1CEE-4DDE-880B-9BB65781C7CE}">
-  <dimension ref="C3:N17"/>
+  <dimension ref="B3:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="I28" zoomScale="87" workbookViewId="0">
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="3.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
     <col min="5" max="6" width="12.77734375" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="9" width="18.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="3:14" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="6" t="s">
+    <row r="3" spans="3:15" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="3:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6" t="s">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="1" t="s">
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="3:14" s="16" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="12" t="s">
+    <row r="5" spans="3:15" s="13" customFormat="1" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="11"/>
+      <c r="J5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="K5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="L5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="M5" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C6" s="8">
+    <row r="6" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C6" s="7">
         <v>4</v>
       </c>
       <c r="D6" s="3">
@@ -2437,27 +2510,28 @@
       <c r="H6" s="2">
         <v>0</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="2"/>
+      <c r="J6" s="2">
         <v>2</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
       </c>
       <c r="K6" s="2">
         <v>0</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="2">
         <v>0</v>
       </c>
-      <c r="M6" s="1">
-        <v>1</v>
+      <c r="M6" s="3">
+        <v>0</v>
       </c>
       <c r="N6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C7" s="8">
+      <c r="O6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C7" s="7">
         <v>6</v>
       </c>
       <c r="D7" s="3">
@@ -2476,27 +2550,28 @@
       <c r="H7" s="2">
         <v>1</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2">
         <v>3</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0</v>
       </c>
       <c r="K7" s="2">
         <v>0</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
         <v>1</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <v>2</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O7" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C8" s="8">
+    <row r="8" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C8" s="7">
         <v>8</v>
       </c>
       <c r="D8" s="3">
@@ -2515,27 +2590,28 @@
       <c r="H8" s="2">
         <v>2</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="2"/>
+      <c r="J8" s="2">
         <v>7</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <v>1</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <v>0</v>
       </c>
-      <c r="L8" s="3">
+      <c r="M8" s="3">
         <v>2</v>
-      </c>
-      <c r="M8" s="1">
-        <v>5</v>
       </c>
       <c r="N8" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C9" s="8">
+      <c r="O8" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C9" s="7">
         <v>10</v>
       </c>
       <c r="D9" s="3">
@@ -2554,27 +2630,28 @@
       <c r="H9" s="2">
         <v>8</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="2"/>
+      <c r="J9" s="2">
         <v>13</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <v>3</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <v>2</v>
       </c>
-      <c r="L9" s="3">
+      <c r="M9" s="3">
         <v>8</v>
-      </c>
-      <c r="M9" s="1">
-        <v>12</v>
       </c>
       <c r="N9" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C10" s="8">
+      <c r="O9" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C10" s="7">
         <v>12</v>
       </c>
       <c r="D10" s="3">
@@ -2593,27 +2670,28 @@
       <c r="H10" s="2">
         <v>21</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="2"/>
+      <c r="J10" s="2">
         <v>35</v>
       </c>
-      <c r="J10" s="2">
+      <c r="K10" s="2">
         <v>15</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>9</v>
       </c>
-      <c r="L10" s="3">
+      <c r="M10" s="3">
         <v>21</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1">
         <v>31</v>
       </c>
-      <c r="N10" s="1">
+      <c r="O10" s="1">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C11" s="8">
+    <row r="11" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C11" s="7">
         <v>14</v>
       </c>
       <c r="D11" s="3">
@@ -2632,27 +2710,28 @@
       <c r="H11" s="2">
         <v>70</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="2"/>
+      <c r="J11" s="2">
         <v>85</v>
       </c>
-      <c r="J11" s="2">
+      <c r="K11" s="2">
         <v>48</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>43</v>
       </c>
-      <c r="L11" s="3">
+      <c r="M11" s="3">
         <v>70</v>
-      </c>
-      <c r="M11" s="1">
-        <v>84</v>
       </c>
       <c r="N11" s="1">
         <v>84</v>
       </c>
-    </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C12" s="8">
+      <c r="O11" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C12" s="7">
         <v>16</v>
       </c>
       <c r="D12" s="3">
@@ -2671,27 +2750,28 @@
       <c r="H12" s="2">
         <v>212</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="2"/>
+      <c r="J12" s="2">
         <v>257</v>
       </c>
-      <c r="J12" s="2">
+      <c r="K12" s="2">
         <v>183</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <v>158</v>
       </c>
-      <c r="L12" s="3">
+      <c r="M12" s="3">
         <v>212</v>
-      </c>
-      <c r="M12" s="1">
-        <v>250</v>
       </c>
       <c r="N12" s="1">
         <v>250</v>
       </c>
-    </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C13" s="8">
+      <c r="O12" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C13" s="7">
         <v>18</v>
       </c>
       <c r="D13" s="3">
@@ -2710,27 +2790,28 @@
       <c r="H13" s="2">
         <v>715</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="2"/>
+      <c r="J13" s="2">
         <v>765</v>
       </c>
-      <c r="J13" s="2">
+      <c r="K13" s="2">
         <v>622</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>602</v>
       </c>
-      <c r="L13" s="3">
+      <c r="M13" s="3">
         <v>715</v>
       </c>
-      <c r="M13" s="1">
+      <c r="N13" s="1">
         <v>762</v>
       </c>
-      <c r="N13" s="1">
+      <c r="O13" s="1">
         <v>764</v>
       </c>
     </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C14" s="8">
+    <row r="14" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C14" s="7">
         <v>20</v>
       </c>
       <c r="D14" s="3">
@@ -2749,27 +2830,28 @@
       <c r="H14" s="2">
         <v>2364</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="2"/>
+      <c r="J14" s="2">
         <v>2518</v>
       </c>
-      <c r="J14" s="2">
+      <c r="K14" s="2">
         <v>2234</v>
       </c>
-      <c r="K14" s="2">
+      <c r="L14" s="2">
         <v>2136</v>
       </c>
-      <c r="L14" s="3">
+      <c r="M14" s="3">
         <v>2364</v>
-      </c>
-      <c r="M14" s="1">
-        <v>2504</v>
       </c>
       <c r="N14" s="1">
         <v>2504</v>
       </c>
-    </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C15" s="8">
+      <c r="O14" s="1">
+        <v>2504</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C15" s="7">
         <v>22</v>
       </c>
       <c r="D15" s="3">
@@ -2788,27 +2870,28 @@
       <c r="H15" s="2">
         <v>8186</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="2"/>
+      <c r="J15" s="2">
         <v>8359</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K15" s="2">
         <v>7800</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
         <v>7721</v>
       </c>
-      <c r="L15" s="3">
+      <c r="M15" s="3">
         <v>8186</v>
-      </c>
-      <c r="M15" s="1">
-        <v>8358</v>
       </c>
       <c r="N15" s="1">
         <v>8358</v>
       </c>
-    </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C16" s="8">
+      <c r="O15" s="1">
+        <v>8358</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C16" s="7">
         <v>24</v>
       </c>
       <c r="D16" s="3">
@@ -2827,27 +2910,28 @@
       <c r="H16" s="2">
         <v>28416</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="2"/>
+      <c r="J16" s="2">
         <v>28968</v>
       </c>
-      <c r="J16" s="2">
+      <c r="K16" s="2">
         <v>27854</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
         <v>27482</v>
       </c>
-      <c r="L16" s="3">
+      <c r="M16" s="3">
         <v>28416</v>
       </c>
-      <c r="M16" s="1">
+      <c r="N16" s="1">
         <v>28928</v>
       </c>
-      <c r="N16" s="1">
+      <c r="O16" s="1">
         <v>28933</v>
       </c>
     </row>
-    <row r="17" spans="3:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="9">
+    <row r="17" spans="2:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="8">
         <v>26</v>
       </c>
       <c r="D17" s="5">
@@ -2866,30 +2950,489 @@
       <c r="H17" s="4">
         <v>100720</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="4"/>
+      <c r="J17" s="4">
         <v>101340</v>
       </c>
-      <c r="J17" s="4">
+      <c r="K17" s="4">
         <v>99134</v>
       </c>
-      <c r="K17" s="4">
+      <c r="L17" s="4">
         <v>98830</v>
       </c>
-      <c r="L17" s="5">
+      <c r="M17" s="5">
         <v>100720</v>
-      </c>
-      <c r="M17" s="1">
-        <v>101339</v>
       </c>
       <c r="N17" s="1">
         <v>101339</v>
       </c>
+      <c r="O17" s="1">
+        <v>101339</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B30" s="13"/>
+      <c r="C30" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="13" t="str">
+        <f>COMPLEX(0,1)</f>
+        <v>i</v>
+      </c>
+      <c r="E30" s="13" t="str">
+        <f>COMPLEX(0,1)</f>
+        <v>i</v>
+      </c>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B31" s="13"/>
+      <c r="C31" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="20">
+        <v>0</v>
+      </c>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20">
+        <f>2*PI()/4</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20">
+        <f>6*PI()/4</f>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="O31" s="20"/>
+      <c r="P31" s="13"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B32" s="13"/>
+      <c r="C32" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="20">
+        <v>1</v>
+      </c>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20">
+        <v>-1</v>
+      </c>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20">
+        <v>1</v>
+      </c>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20">
+        <v>-1</v>
+      </c>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="13"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B33" s="13"/>
+      <c r="C33" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="13">
+        <v>1</v>
+      </c>
+      <c r="E33" s="13">
+        <v>-1</v>
+      </c>
+      <c r="F33" s="13">
+        <v>1</v>
+      </c>
+      <c r="G33" s="13">
+        <v>-1</v>
+      </c>
+      <c r="H33" s="13">
+        <v>1</v>
+      </c>
+      <c r="I33" s="13">
+        <v>-1</v>
+      </c>
+      <c r="J33" s="13">
+        <v>1</v>
+      </c>
+      <c r="K33" s="13">
+        <v>-1</v>
+      </c>
+      <c r="L33" s="13">
+        <v>1</v>
+      </c>
+      <c r="M33" s="13">
+        <v>-1</v>
+      </c>
+      <c r="N33" s="13">
+        <v>1</v>
+      </c>
+      <c r="O33" s="13">
+        <v>-1</v>
+      </c>
+      <c r="P33" s="13"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B34" s="13">
+        <v>0</v>
+      </c>
+      <c r="C34" s="21" t="str">
+        <f t="shared" ref="C34:C37" si="1">DEC2BIN(B34,4)</f>
+        <v>0000</v>
+      </c>
+      <c r="D34" s="13">
+        <v>8</v>
+      </c>
+      <c r="E34" s="13">
+        <v>8</v>
+      </c>
+      <c r="F34" s="13">
+        <v>0</v>
+      </c>
+      <c r="G34" s="13">
+        <v>0</v>
+      </c>
+      <c r="H34" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K34" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="L34" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M34" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="N34" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="O34" s="13">
+        <v>0</v>
+      </c>
+      <c r="P34" s="13"/>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B35" s="13">
+        <v>1</v>
+      </c>
+      <c r="C35" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>0001</v>
+      </c>
+      <c r="D35" s="13">
+        <v>2</v>
+      </c>
+      <c r="E35" s="13">
+        <v>2</v>
+      </c>
+      <c r="F35" s="13">
+        <v>0</v>
+      </c>
+      <c r="G35" s="13">
+        <v>0</v>
+      </c>
+      <c r="H35" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K35" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="L35" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="M35" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="N35" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="O35" s="13">
+        <v>1</v>
+      </c>
+      <c r="P35" s="13"/>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B36" s="13">
+        <v>3</v>
+      </c>
+      <c r="C36" s="21" t="str">
+        <f t="shared" si="1"/>
+        <v>0011</v>
+      </c>
+      <c r="D36" s="13">
+        <v>4</v>
+      </c>
+      <c r="E36" s="13">
+        <v>0</v>
+      </c>
+      <c r="F36" s="13">
+        <v>0</v>
+      </c>
+      <c r="G36" s="13">
+        <v>0</v>
+      </c>
+      <c r="H36" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="K36" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="L36" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M36" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="N36" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="O36" s="13">
+        <v>2</v>
+      </c>
+      <c r="P36" s="13"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B37" s="23">
+        <v>5</v>
+      </c>
+      <c r="C37" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>0101</v>
+      </c>
+      <c r="D37" s="23">
+        <v>8</v>
+      </c>
+      <c r="E37" s="23">
+        <v>0</v>
+      </c>
+      <c r="F37" s="23">
+        <v>0</v>
+      </c>
+      <c r="G37" s="23">
+        <v>0</v>
+      </c>
+      <c r="H37" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="J37" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="K37" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="L37" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="M37" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="N37" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="O37" s="23">
+        <v>0</v>
+      </c>
+      <c r="P37" s="13"/>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B38" s="13"/>
+      <c r="C38" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="27">
+        <f>4</f>
+        <v>4</v>
+      </c>
+      <c r="E38" s="27">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="F38" s="27">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="27">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="27">
+        <v>1</v>
+      </c>
+      <c r="I38" s="27">
+        <v>2</v>
+      </c>
+      <c r="J38" s="27">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="K38" s="27">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="27">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="M38" s="27">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="N38" s="27">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="O38" s="27">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="P38" s="26">
+        <f>SUM(D38:O38)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C39" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="1">
+        <v>4</v>
+      </c>
+      <c r="E39" s="1">
+        <v>2</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J39" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K39" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="L39" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="M39" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="N39" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O39" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C41" s="19"/>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C42" s="19"/>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C43" s="19"/>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C44" s="19"/>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C45" s="19"/>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C46" s="19"/>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C47" s="19"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="18"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C50" s="18"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C51" s="18"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C52" s="18"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C53" s="18"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C54" s="18"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C55" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="13">
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="N31:O31"/>
     <mergeCell ref="E4:H4"/>
-    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="J4:M4"/>
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H31:I31"/>
   </mergeCells>
   <conditionalFormatting sqref="F19">
     <cfRule type="dataBar" priority="1">

</xml_diff>